<commit_message>
sensitivity module bug fixed
</commit_message>
<xml_diff>
--- a/CVX_Kenya/New Code/Ecopulpers.xlsx
+++ b/CVX_Kenya/New Code/Ecopulpers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\New Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A16A0D-20BC-4D37-ABA2-68408FFBEF32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BF145F-66FF-44EB-AC10-9906CC84C091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="250">
   <si>
     <t>level_row</t>
   </si>
@@ -777,9 +777,6 @@
   </si>
   <si>
     <t>300-600,50</t>
-  </si>
-  <si>
-    <t>0%-2.5%,0.5%</t>
   </si>
   <si>
     <t>Green Water</t>
@@ -798,11 +795,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1079,9 +1075,6 @@
     <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1102,9 +1095,6 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1116,6 +1106,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1131,6 +1124,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1483,8 +1479,8 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
-        <v>247</v>
+      <c r="B2" s="45" t="s">
+        <v>246</v>
       </c>
       <c r="C2" t="s">
         <v>92</v>
@@ -1492,7 +1488,7 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="44">
+      <c r="E2" s="43">
         <f>main!C34</f>
         <v>-2.5504753816423371E-2</v>
       </c>
@@ -1510,7 +1506,7 @@
       <c r="D3" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E3" s="45">
+      <c r="E3" s="44">
         <f>main!C31</f>
         <v>1.9446613275375006E-2</v>
       </c>
@@ -1539,7 +1535,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1634,7 +1630,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1670,7 +1666,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1694,7 +1690,7 @@
       </c>
       <c r="G2" s="5">
         <f>-main!C29</f>
-        <v>-5.3915624999999997E-3</v>
+        <v>-0.35943749999999997</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>218</v>
@@ -1719,7 +1715,7 @@
       <c r="F3" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="G3" s="51">
+      <c r="G3" s="49">
         <f>main!C30/100</f>
         <v>8.066743284600001E-3</v>
       </c>
@@ -1746,7 +1742,7 @@
       <c r="F4" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="G4" s="39">
+      <c r="G4" s="38">
         <f>main!C33</f>
         <v>3.1949999999999998</v>
       </c>
@@ -1803,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1834,7 +1830,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>240</v>
@@ -2612,8 +2608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2640,20 +2636,20 @@
       <c r="D1" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="48" t="s">
         <v>242</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="I1" s="50" t="s">
-        <v>248</v>
+      <c r="I1" s="48" t="s">
+        <v>247</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>177</v>
@@ -2663,7 +2659,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="54" t="s">
         <v>172</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -2681,12 +2677,12 @@
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
       <c r="J2" s="17"/>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="37" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="56"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="16" t="s">
         <v>173</v>
       </c>
@@ -2705,7 +2701,7 @@
       <c r="K3" s="17"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="56"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="16" t="s">
         <v>237</v>
       </c>
@@ -2724,7 +2720,7 @@
       <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="56"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="16" t="s">
         <v>189</v>
       </c>
@@ -2743,11 +2739,11 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="56"/>
-      <c r="B6" s="36" t="s">
+      <c r="A6" s="55"/>
+      <c r="B6" s="35" t="s">
         <v>231</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="36">
         <v>0.27</v>
       </c>
       <c r="D6" s="23" t="s">
@@ -2759,12 +2755,12 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="17"/>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="37" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="56"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="16" t="s">
         <v>191</v>
       </c>
@@ -2781,7 +2777,7 @@
       <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="56"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="16" t="s">
         <v>194</v>
       </c>
@@ -2800,7 +2796,7 @@
       <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="56"/>
+      <c r="A9" s="55"/>
       <c r="B9" s="16" t="s">
         <v>198</v>
       </c>
@@ -2819,7 +2815,7 @@
       <c r="K9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="56"/>
+      <c r="A10" s="55"/>
       <c r="B10" s="16" t="s">
         <v>201</v>
       </c>
@@ -2836,7 +2832,7 @@
       <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="56"/>
+      <c r="A11" s="55"/>
       <c r="B11" s="16" t="s">
         <v>200</v>
       </c>
@@ -2855,7 +2851,7 @@
       <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="56"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="16" t="s">
         <v>207</v>
       </c>
@@ -2874,7 +2870,7 @@
       <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="56"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="16" t="s">
         <v>209</v>
       </c>
@@ -2893,7 +2889,7 @@
       <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="56"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="16" t="s">
         <v>210</v>
       </c>
@@ -2904,7 +2900,7 @@
         <v>211</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="F14" s="23">
         <v>0.107</v>
@@ -2916,13 +2912,13 @@
         <v>1E-3</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="56"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="16" t="s">
         <v>186</v>
       </c>
@@ -2939,7 +2935,7 @@
       <c r="K15" s="17"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="56"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="16" t="s">
         <v>224</v>
       </c>
@@ -2958,26 +2954,26 @@
       <c r="K16" s="17"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="39" t="s">
         <v>220</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="46">
         <v>639</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="53" t="s">
         <v>180</v>
       </c>
       <c r="B18" s="15" t="s">
@@ -2996,7 +2992,7 @@
       <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="15" t="s">
         <v>188</v>
       </c>
@@ -3015,26 +3011,35 @@
       <c r="K19" s="20"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="C20" s="46">
-        <v>1.4999999999999999E-2</v>
+      <c r="C20" s="50">
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
+        <v>244</v>
+      </c>
+      <c r="F20" s="24">
+        <v>0</v>
+      </c>
+      <c r="G20" s="24">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H20" s="24">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>248</v>
+      </c>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="52" t="s">
         <v>181</v>
       </c>
       <c r="B21" s="21" t="s">
@@ -3056,7 +3061,7 @@
       <c r="K21" s="22"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="53"/>
+      <c r="A22" s="52"/>
       <c r="B22" s="28" t="s">
         <v>222</v>
       </c>
@@ -3074,13 +3079,13 @@
       <c r="K22" s="22"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="53"/>
+      <c r="A23" s="52"/>
       <c r="B23" s="28" t="s">
         <v>185</v>
       </c>
       <c r="C23" s="33">
         <f>C20*C17/C22</f>
-        <v>5.3915624999999997E-3</v>
+        <v>0.35943749999999997</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
@@ -3092,7 +3097,7 @@
       <c r="K23" s="22"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="53"/>
+      <c r="A24" s="52"/>
       <c r="B24" s="21" t="s">
         <v>204</v>
       </c>
@@ -3112,7 +3117,7 @@
       <c r="K24" s="22"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="53"/>
+      <c r="A25" s="52"/>
       <c r="B25" s="21" t="s">
         <v>230</v>
       </c>
@@ -3132,7 +3137,7 @@
       <c r="K25" s="22"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="53"/>
+      <c r="A26" s="52"/>
       <c r="B26" s="21" t="s">
         <v>206</v>
       </c>
@@ -3152,7 +3157,7 @@
       <c r="K26" s="22"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="51" t="s">
         <v>182</v>
       </c>
       <c r="B27" s="18" t="s">
@@ -3176,7 +3181,7 @@
       <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="52"/>
+      <c r="A28" s="51"/>
       <c r="B28" s="18" t="s">
         <v>184</v>
       </c>
@@ -3198,13 +3203,13 @@
       <c r="K28" s="19"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="52"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C29" s="35">
+      <c r="C29" s="56">
         <f>C23</f>
-        <v>5.3915624999999997E-3</v>
+        <v>0.35943749999999997</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>227</v>
@@ -3220,7 +3225,7 @@
       <c r="K29" s="19"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="52"/>
+      <c r="A30" s="51"/>
       <c r="B30" s="18" t="s">
         <v>192</v>
       </c>
@@ -3242,7 +3247,7 @@
       <c r="K30" s="19"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="52"/>
+      <c r="A31" s="51"/>
       <c r="B31" s="18" t="s">
         <v>229</v>
       </c>
@@ -3264,7 +3269,7 @@
       <c r="K31" s="19"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="52"/>
+      <c r="A32" s="51"/>
       <c r="B32" s="18" t="s">
         <v>226</v>
       </c>
@@ -3286,7 +3291,7 @@
       <c r="K32" s="19"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="52"/>
+      <c r="A33" s="51"/>
       <c r="B33" s="18" t="s">
         <v>238</v>
       </c>
@@ -3308,7 +3313,7 @@
       <c r="K33" s="19"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="52"/>
+      <c r="A34" s="51"/>
       <c r="B34" s="18" t="s">
         <v>193</v>
       </c>

</xml_diff>